<commit_message>
Complete Mail Scripts Beta Version
</commit_message>
<xml_diff>
--- a/Input_parameters.xlsx
+++ b/Input_parameters.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>부문</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -30,9 +30,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>안녕하세요.
-한국생산성본부 신백균입니다.
-어쩌구 저쩌구 테스트 메시지입니다.</t>
+    <t>설명 주저리 주저리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제목</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매·자재</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -42,18 +48,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>설명 주저리 주저리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>구매·자재</t>
-  </si>
-  <si>
-    <t>품질</t>
+    <t>안녕하세요.
+한국생산성본부 신백균 위원입니다.
+하기의 교육과정과 관련하여 강의 정보 안내 및 일정표, 수강생 명단을 송부하오니
+꼭 확인해 주시기 바랍니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -409,7 +407,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -419,12 +417,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -432,18 +430,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.45">
@@ -451,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Text alignment and font size
</commit_message>
<xml_diff>
--- a/Input_parameters.xlsx
+++ b/Input_parameters.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="스크립트" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>부문</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -27,10 +27,6 @@
   </si>
   <si>
     <t>끝인사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>설명 주저리 주저리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -52,6 +48,22 @@
 한국생산성본부 신백균 위원입니다.
 하기의 교육과정과 관련하여 강의 정보 안내 및 일정표, 수강생 명단을 송부하오니
 꼭 확인해 주시기 바랍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강사 메일 스크립트 자동 생성 Input Parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정표 원본파일명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019일정계획표(2019.08.02).xlsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -83,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -91,16 +103,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -404,50 +435,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.45">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>